<commit_message>
Change client data structures and modify inspection coverage plot
</commit_message>
<xml_diff>
--- a/Documentation/Reward_Parameters.xlsx
+++ b/Documentation/Reward_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\MATLAB\SimscapeSatelliteInspection\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ED0F66-6748-413E-A6A5-583B0EA2816C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBFA7C0-55E2-41A2-888B-4D51A80D0AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1248" yWindow="972" windowWidth="21600" windowHeight="11388" activeTab="2" xr2:uid="{21604E66-B88B-4810-977B-379932FB21BA}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="9024" firstSheet="2" activeTab="6" xr2:uid="{21604E66-B88B-4810-977B-379932FB21BA}"/>
   </bookViews>
   <sheets>
     <sheet name="EE_Position" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="EE_Orientation" sheetId="6" r:id="rId4"/>
     <sheet name="Control" sheetId="7" r:id="rId5"/>
     <sheet name="Smoothness" sheetId="9" r:id="rId6"/>
+    <sheet name="Coverage" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Bias</t>
   </si>
@@ -51,6 +52,24 @@
   </si>
   <si>
     <t>Power</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>bias</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>exp</t>
   </si>
 </sst>
 </file>
@@ -11213,6 +11232,1041 @@
                   <a:t> Error (m)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595611320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="595611320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Reward Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595595640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Coverage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Reward</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Coverage!$A$4:$A$303</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="300"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Coverage!$B$4:$B$303</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="300"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8162976389793695E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6655846490923683E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5484602155080109E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4655344063813578E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4174283705210415E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11404774538646767</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13428216828302508</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15488410852491374</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17586024132099976</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.19721736312181015</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21896239382164273</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24110237900067166</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26364449220777786</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28659603728484062</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3099644507332473</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.33375730412338456</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.35798230654789265</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.38264730711947958</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.40776029751410259</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.43332941456034035</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.4593629428757966</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.48586931755138973</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.51285712688439467</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.54033511516112709</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.56831218549016893</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.59679740268705261</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.62579999621134164</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.65532936315705514</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.68539507129740884</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.71600686218485854</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.74717465430744623</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.77890854630247852</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.81121882022857283</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.84411594489713448</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.87761057926434316</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.91171357588474833</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.94643598442759136</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.98178905525699478</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0177842430771791</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0544332106438881</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0917478325432208</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.1297401990391056</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.1684226199906478</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.2078076288406328</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.2479079866764717</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.288736686364905</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.3303069567618055</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.3726322669984423</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.4157263308455978</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.4596031111569499</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.5042768243931568</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.5497619452281173</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.5960732112388905</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.6432256276807986</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.6912344723492625</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.7401153005299417</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.7898839500387789</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.8405565463535978</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.8921495078388926</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9446795510655241</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.9981636962270355</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.052619272654344</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.1080639244305943</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.1645156161079973</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.2219926385285005</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.2805136147501828</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.3400975060812876</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.4007636182238512</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.4625316075289199</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.5254214873653824</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5894536346044714</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.6546487962220517</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.7210280960208211</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.7886130414746066</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.8574255306969745</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.9274878595364116</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.998822728800373</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.0714532516105448</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.1454029608916967</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.2206958169965532</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.2973562154691631</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.3754089949492627</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.4548794452202172</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.5357933154031294</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.6181768222997812</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.7020566588871047</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.7874600029659442</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.8744145259668965</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.9629484019161012</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.0530903165638676</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.144869476679113</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.2383156195126066</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.3334590224321019</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.4303305127324677</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.5289614776240041</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.6293838744021683</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4.7316302408020201</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4.8357337055407354</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4.9417279990515954</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>5.0496474644129465</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E38-4461-8E9A-141CF86090EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="595595640"/>
+        <c:axId val="595611320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="595595640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent of Faces Covered</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -11656,6 +12710,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -14791,6 +15885,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15027,6 +16637,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94DFCC81-BD7A-4363-A9E9-E2C70CA8BA08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFED3F0A-9197-44C3-AA6F-93371F014F57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21739,7 +23392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D3764F-0861-407A-B11B-13C66D84A4F6}">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -29954,4 +31607,965 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA46DC3-B71F-4361-89CF-C6900FE3717A}">
+  <dimension ref="A1:D104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1.8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f>$C$3*EXP($B$3*A4)+$D$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.01</v>
+      </c>
+      <c r="B5">
+        <f>$C$3*EXP($B$3*A5)+$D$3</f>
+        <v>1.8162976389793695E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.02</v>
+      </c>
+      <c r="B6">
+        <f>$C$3*EXP($B$3*A6)+$D$3</f>
+        <v>3.6655846490923683E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.03</v>
+      </c>
+      <c r="B7">
+        <f>$C$3*EXP($B$3*A7)+$D$3</f>
+        <v>5.5484602155080109E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.04</v>
+      </c>
+      <c r="B8">
+        <f>$C$3*EXP($B$3*A8)+$D$3</f>
+        <v>7.4655344063813578E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.05</v>
+      </c>
+      <c r="B9">
+        <f>$C$3*EXP($B$3*A9)+$D$3</f>
+        <v>9.4174283705210415E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.06</v>
+      </c>
+      <c r="B10">
+        <f>$C$3*EXP($B$3*A10)+$D$3</f>
+        <v>0.11404774538646767</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B11">
+        <f>$C$3*EXP($B$3*A11)+$D$3</f>
+        <v>0.13428216828302508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.08</v>
+      </c>
+      <c r="B12">
+        <f>$C$3*EXP($B$3*A12)+$D$3</f>
+        <v>0.15488410852491374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.09</v>
+      </c>
+      <c r="B13">
+        <f>$C$3*EXP($B$3*A13)+$D$3</f>
+        <v>0.17586024132099976</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.1</v>
+      </c>
+      <c r="B14">
+        <f>$C$3*EXP($B$3*A14)+$D$3</f>
+        <v>0.19721736312181015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.11</v>
+      </c>
+      <c r="B15">
+        <f>$C$3*EXP($B$3*A15)+$D$3</f>
+        <v>0.21896239382164273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.12</v>
+      </c>
+      <c r="B16">
+        <f>$C$3*EXP($B$3*A16)+$D$3</f>
+        <v>0.24110237900067166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.13</v>
+      </c>
+      <c r="B17">
+        <f>$C$3*EXP($B$3*A17)+$D$3</f>
+        <v>0.26364449220777786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B18">
+        <f>$C$3*EXP($B$3*A18)+$D$3</f>
+        <v>0.28659603728484062</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.15</v>
+      </c>
+      <c r="B19">
+        <f>$C$3*EXP($B$3*A19)+$D$3</f>
+        <v>0.3099644507332473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.16</v>
+      </c>
+      <c r="B20">
+        <f>$C$3*EXP($B$3*A20)+$D$3</f>
+        <v>0.33375730412338456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0.17</v>
+      </c>
+      <c r="B21">
+        <f>$C$3*EXP($B$3*A21)+$D$3</f>
+        <v>0.35798230654789265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0.18</v>
+      </c>
+      <c r="B22">
+        <f>$C$3*EXP($B$3*A22)+$D$3</f>
+        <v>0.38264730711947958</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0.19</v>
+      </c>
+      <c r="B23">
+        <f>$C$3*EXP($B$3*A23)+$D$3</f>
+        <v>0.40776029751410259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0.2</v>
+      </c>
+      <c r="B24">
+        <f>$C$3*EXP($B$3*A24)+$D$3</f>
+        <v>0.43332941456034035</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0.21</v>
+      </c>
+      <c r="B25">
+        <f>$C$3*EXP($B$3*A25)+$D$3</f>
+        <v>0.4593629428757966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0.22</v>
+      </c>
+      <c r="B26">
+        <f>$C$3*EXP($B$3*A26)+$D$3</f>
+        <v>0.48586931755138973</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.23</v>
+      </c>
+      <c r="B27">
+        <f>$C$3*EXP($B$3*A27)+$D$3</f>
+        <v>0.51285712688439467</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.24</v>
+      </c>
+      <c r="B28">
+        <f>$C$3*EXP($B$3*A28)+$D$3</f>
+        <v>0.54033511516112709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.25</v>
+      </c>
+      <c r="B29">
+        <f>$C$3*EXP($B$3*A29)+$D$3</f>
+        <v>0.56831218549016893</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.26</v>
+      </c>
+      <c r="B30">
+        <f>$C$3*EXP($B$3*A30)+$D$3</f>
+        <v>0.59679740268705261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.27</v>
+      </c>
+      <c r="B31">
+        <f>$C$3*EXP($B$3*A31)+$D$3</f>
+        <v>0.62579999621134164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B32">
+        <f>$C$3*EXP($B$3*A32)+$D$3</f>
+        <v>0.65532936315705514</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B33">
+        <f>$C$3*EXP($B$3*A33)+$D$3</f>
+        <v>0.68539507129740884</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.3</v>
+      </c>
+      <c r="B34">
+        <f>$C$3*EXP($B$3*A34)+$D$3</f>
+        <v>0.71600686218485854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0.31</v>
+      </c>
+      <c r="B35">
+        <f>$C$3*EXP($B$3*A35)+$D$3</f>
+        <v>0.74717465430744623</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.32</v>
+      </c>
+      <c r="B36">
+        <f>$C$3*EXP($B$3*A36)+$D$3</f>
+        <v>0.77890854630247852</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0.33</v>
+      </c>
+      <c r="B37">
+        <f>$C$3*EXP($B$3*A37)+$D$3</f>
+        <v>0.81121882022857283</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.34</v>
+      </c>
+      <c r="B38">
+        <f>$C$3*EXP($B$3*A38)+$D$3</f>
+        <v>0.84411594489713448</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0.35</v>
+      </c>
+      <c r="B39">
+        <f>$C$3*EXP($B$3*A39)+$D$3</f>
+        <v>0.87761057926434316</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0.36</v>
+      </c>
+      <c r="B40">
+        <f>$C$3*EXP($B$3*A40)+$D$3</f>
+        <v>0.91171357588474833</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0.37</v>
+      </c>
+      <c r="B41">
+        <f>$C$3*EXP($B$3*A41)+$D$3</f>
+        <v>0.94643598442759136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0.38</v>
+      </c>
+      <c r="B42">
+        <f>$C$3*EXP($B$3*A42)+$D$3</f>
+        <v>0.98178905525699478</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0.39</v>
+      </c>
+      <c r="B43">
+        <f>$C$3*EXP($B$3*A43)+$D$3</f>
+        <v>1.0177842430771791</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0.4</v>
+      </c>
+      <c r="B44">
+        <f>$C$3*EXP($B$3*A44)+$D$3</f>
+        <v>1.0544332106438881</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0.41</v>
+      </c>
+      <c r="B45">
+        <f>$C$3*EXP($B$3*A45)+$D$3</f>
+        <v>1.0917478325432208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0.42</v>
+      </c>
+      <c r="B46">
+        <f>$C$3*EXP($B$3*A46)+$D$3</f>
+        <v>1.1297401990391056</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0.43</v>
+      </c>
+      <c r="B47">
+        <f>$C$3*EXP($B$3*A47)+$D$3</f>
+        <v>1.1684226199906478</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0.44</v>
+      </c>
+      <c r="B48">
+        <f>$C$3*EXP($B$3*A48)+$D$3</f>
+        <v>1.2078076288406328</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0.45</v>
+      </c>
+      <c r="B49">
+        <f>$C$3*EXP($B$3*A49)+$D$3</f>
+        <v>1.2479079866764717</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0.46</v>
+      </c>
+      <c r="B50">
+        <f>$C$3*EXP($B$3*A50)+$D$3</f>
+        <v>1.288736686364905</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0.47</v>
+      </c>
+      <c r="B51">
+        <f>$C$3*EXP($B$3*A51)+$D$3</f>
+        <v>1.3303069567618055</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0.48</v>
+      </c>
+      <c r="B52">
+        <f>$C$3*EXP($B$3*A52)+$D$3</f>
+        <v>1.3726322669984423</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0.49</v>
+      </c>
+      <c r="B53">
+        <f>$C$3*EXP($B$3*A53)+$D$3</f>
+        <v>1.4157263308455978</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0.5</v>
+      </c>
+      <c r="B54">
+        <f>$C$3*EXP($B$3*A54)+$D$3</f>
+        <v>1.4596031111569499</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0.51</v>
+      </c>
+      <c r="B55">
+        <f>$C$3*EXP($B$3*A55)+$D$3</f>
+        <v>1.5042768243931568</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0.52</v>
+      </c>
+      <c r="B56">
+        <f>$C$3*EXP($B$3*A56)+$D$3</f>
+        <v>1.5497619452281173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0.53</v>
+      </c>
+      <c r="B57">
+        <f>$C$3*EXP($B$3*A57)+$D$3</f>
+        <v>1.5960732112388905</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0.54</v>
+      </c>
+      <c r="B58">
+        <f>$C$3*EXP($B$3*A58)+$D$3</f>
+        <v>1.6432256276807986</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B59">
+        <f>$C$3*EXP($B$3*A59)+$D$3</f>
+        <v>1.6912344723492625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B60">
+        <f>$C$3*EXP($B$3*A60)+$D$3</f>
+        <v>1.7401153005299417</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="B61">
+        <f>$C$3*EXP($B$3*A61)+$D$3</f>
+        <v>1.7898839500387789</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B62">
+        <f>$C$3*EXP($B$3*A62)+$D$3</f>
+        <v>1.8405565463535978</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0.59</v>
+      </c>
+      <c r="B63">
+        <f>$C$3*EXP($B$3*A63)+$D$3</f>
+        <v>1.8921495078388926</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0.6</v>
+      </c>
+      <c r="B64">
+        <f>$C$3*EXP($B$3*A64)+$D$3</f>
+        <v>1.9446795510655241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0.61</v>
+      </c>
+      <c r="B65">
+        <f>$C$3*EXP($B$3*A65)+$D$3</f>
+        <v>1.9981636962270355</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0.62</v>
+      </c>
+      <c r="B66">
+        <f>$C$3*EXP($B$3*A66)+$D$3</f>
+        <v>2.052619272654344</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0.63</v>
+      </c>
+      <c r="B67">
+        <f>$C$3*EXP($B$3*A67)+$D$3</f>
+        <v>2.1080639244305943</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0.64</v>
+      </c>
+      <c r="B68">
+        <f>$C$3*EXP($B$3*A68)+$D$3</f>
+        <v>2.1645156161079973</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0.65</v>
+      </c>
+      <c r="B69">
+        <f>$C$3*EXP($B$3*A69)+$D$3</f>
+        <v>2.2219926385285005</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0.66</v>
+      </c>
+      <c r="B70">
+        <f>$C$3*EXP($B$3*A70)+$D$3</f>
+        <v>2.2805136147501828</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0.67</v>
+      </c>
+      <c r="B71">
+        <f>$C$3*EXP($B$3*A71)+$D$3</f>
+        <v>2.3400975060812876</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0.68</v>
+      </c>
+      <c r="B72">
+        <f>$C$3*EXP($B$3*A72)+$D$3</f>
+        <v>2.4007636182238512</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0.69</v>
+      </c>
+      <c r="B73">
+        <f>$C$3*EXP($B$3*A73)+$D$3</f>
+        <v>2.4625316075289199</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0.7</v>
+      </c>
+      <c r="B74">
+        <f>$C$3*EXP($B$3*A74)+$D$3</f>
+        <v>2.5254214873653824</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0.71</v>
+      </c>
+      <c r="B75">
+        <f>$C$3*EXP($B$3*A75)+$D$3</f>
+        <v>2.5894536346044714</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0.72</v>
+      </c>
+      <c r="B76">
+        <f>$C$3*EXP($B$3*A76)+$D$3</f>
+        <v>2.6546487962220517</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0.73</v>
+      </c>
+      <c r="B77">
+        <f>$C$3*EXP($B$3*A77)+$D$3</f>
+        <v>2.7210280960208211</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0.74</v>
+      </c>
+      <c r="B78">
+        <f>$C$3*EXP($B$3*A78)+$D$3</f>
+        <v>2.7886130414746066</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0.75</v>
+      </c>
+      <c r="B79">
+        <f>$C$3*EXP($B$3*A79)+$D$3</f>
+        <v>2.8574255306969745</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0.76</v>
+      </c>
+      <c r="B80">
+        <f>$C$3*EXP($B$3*A80)+$D$3</f>
+        <v>2.9274878595364116</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0.77</v>
+      </c>
+      <c r="B81">
+        <f>$C$3*EXP($B$3*A81)+$D$3</f>
+        <v>2.998822728800373</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0.78</v>
+      </c>
+      <c r="B82">
+        <f>$C$3*EXP($B$3*A82)+$D$3</f>
+        <v>3.0714532516105448</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0.79</v>
+      </c>
+      <c r="B83">
+        <f>$C$3*EXP($B$3*A83)+$D$3</f>
+        <v>3.1454029608916967</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0.8</v>
+      </c>
+      <c r="B84">
+        <f>$C$3*EXP($B$3*A84)+$D$3</f>
+        <v>3.2206958169965532</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0.81</v>
+      </c>
+      <c r="B85">
+        <f>$C$3*EXP($B$3*A85)+$D$3</f>
+        <v>3.2973562154691631</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0.82</v>
+      </c>
+      <c r="B86">
+        <f>$C$3*EXP($B$3*A86)+$D$3</f>
+        <v>3.3754089949492627</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0.83</v>
+      </c>
+      <c r="B87">
+        <f>$C$3*EXP($B$3*A87)+$D$3</f>
+        <v>3.4548794452202172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0.84</v>
+      </c>
+      <c r="B88">
+        <f>$C$3*EXP($B$3*A88)+$D$3</f>
+        <v>3.5357933154031294</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0.85</v>
+      </c>
+      <c r="B89">
+        <f>$C$3*EXP($B$3*A89)+$D$3</f>
+        <v>3.6181768222997812</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0.86</v>
+      </c>
+      <c r="B90">
+        <f>$C$3*EXP($B$3*A90)+$D$3</f>
+        <v>3.7020566588871047</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0.87</v>
+      </c>
+      <c r="B91">
+        <f>$C$3*EXP($B$3*A91)+$D$3</f>
+        <v>3.7874600029659442</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0.88</v>
+      </c>
+      <c r="B92">
+        <f>$C$3*EXP($B$3*A92)+$D$3</f>
+        <v>3.8744145259668965</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0.89</v>
+      </c>
+      <c r="B93">
+        <f>$C$3*EXP($B$3*A93)+$D$3</f>
+        <v>3.9629484019161012</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0.9</v>
+      </c>
+      <c r="B94">
+        <f>$C$3*EXP($B$3*A94)+$D$3</f>
+        <v>4.0530903165638676</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0.91</v>
+      </c>
+      <c r="B95">
+        <f>$C$3*EXP($B$3*A95)+$D$3</f>
+        <v>4.144869476679113</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0.92</v>
+      </c>
+      <c r="B96">
+        <f>$C$3*EXP($B$3*A96)+$D$3</f>
+        <v>4.2383156195126066</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0.93</v>
+      </c>
+      <c r="B97">
+        <f>$C$3*EXP($B$3*A97)+$D$3</f>
+        <v>4.3334590224321019</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0.94</v>
+      </c>
+      <c r="B98">
+        <f>$C$3*EXP($B$3*A98)+$D$3</f>
+        <v>4.4303305127324677</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0.95</v>
+      </c>
+      <c r="B99">
+        <f>$C$3*EXP($B$3*A99)+$D$3</f>
+        <v>4.5289614776240041</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0.96</v>
+      </c>
+      <c r="B100">
+        <f>$C$3*EXP($B$3*A100)+$D$3</f>
+        <v>4.6293838744021683</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0.97</v>
+      </c>
+      <c r="B101">
+        <f>$C$3*EXP($B$3*A101)+$D$3</f>
+        <v>4.7316302408020201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>0.98</v>
+      </c>
+      <c r="B102">
+        <f>$C$3*EXP($B$3*A102)+$D$3</f>
+        <v>4.8357337055407354</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>0.99</v>
+      </c>
+      <c r="B103">
+        <f>$C$3*EXP($B$3*A103)+$D$3</f>
+        <v>4.9417279990515954</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <f>$C$3*EXP($B$3*A104)+$D$3</f>
+        <v>5.0496474644129465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>